<commit_message>
Se trabaja carga en Excel modulo Empleado, se agrega ID Areas y Empleados
</commit_message>
<xml_diff>
--- a/storage/app/public/exportExcel/empleado.xlsx
+++ b/storage/app/public/exportExcel/empleado.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosa.flores\Downloads\plantillas Excel (1)\plantillas Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro.garcia\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B002FBB-B323-4584-861F-893C4560FDD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5959EF14-A05B-467D-8EAA-947F521265DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6D05F6C6-55E0-4173-9190-01B85D70B50B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{88EA818E-9576-4B44-B641-A3E0A6393630}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,27 +35,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Nombre1</t>
-  </si>
-  <si>
-    <t>02/14/2019</t>
-  </si>
-  <si>
-    <t>genero1</t>
-  </si>
-  <si>
-    <t>estatus1</t>
-  </si>
-  <si>
-    <t>emal1@teste.com</t>
-  </si>
-  <si>
-    <t>Direccion1</t>
-  </si>
-  <si>
-    <t>testststs</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Numero Empleado</t>
+  </si>
+  <si>
+    <t>Area ID</t>
+  </si>
+  <si>
+    <t>Jefe InmediatoID</t>
+  </si>
+  <si>
+    <t>Puesto ID</t>
+  </si>
+  <si>
+    <t>Nivel Jerarquico ID</t>
+  </si>
+  <si>
+    <t>Genero (H/M)</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Telefono Movil</t>
+  </si>
+  <si>
+    <t>Telefono Fijo</t>
+  </si>
+  <si>
+    <t>Sede ID</t>
+  </si>
+  <si>
+    <t>Direccion</t>
+  </si>
+  <si>
+    <t>Fecha Ingreso DD-MM-AAAA</t>
+  </si>
+  <si>
+    <t>Cumpleaños DD-MM-AAAA</t>
   </si>
 </sst>
 </file>
@@ -70,9 +92,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -95,17 +117,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -417,77 +436,79 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA26AED4-9A36-4B16-BF45-999BB7E21237}">
-  <dimension ref="A1:Q1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B05BADD-88A8-4ADB-B3DD-28048BFEB69B}">
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.08984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>90</v>
-      </c>
-      <c r="C1">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1">
-        <v>3</v>
-      </c>
-      <c r="F1">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" t="s">
-        <v>3</v>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1">
-        <v>11111111111</v>
-      </c>
-      <c r="L1">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1">
-        <v>1</v>
-      </c>
-      <c r="N1">
-        <v>2</v>
-      </c>
-      <c r="O1" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1" s="2">
-        <v>35126</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>6</v>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J1" r:id="rId1" xr:uid="{5347923E-F4AD-4DE5-99B6-B1ED6B492616}"/>
+    <hyperlink ref="J1" r:id="rId1" display="emal1@teste.com" xr:uid="{761D19AF-E63F-4C5B-8DD0-BE98D86CD221}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>